<commit_message>
modifica Claims della chiamata al gtw
inserimento nuovi file dopo modifica Claims(appId,appVersion,appVendor) della chiamata al gtw
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-RAD/3.15.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-RAD/3.15.0.0/report-checklist.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$240</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$240</definedName>
   </definedNames>
   <calcPr/>
@@ -313,13 +313,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-10-12T14:29:56:00Z</t>
-  </si>
-  <si>
-    <t>63ad8feafd0db96d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.801d325d3027b464d1db4e5495ea0b5e952d9150cc84acb2d031010f87f28aa2.1dfaded450^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-10-18T13:00:40:00Z</t>
+  </si>
+  <si>
+    <t>41f8cf7b72e3d992</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.812d16869f3171178394d5957a9d4b9fe359a3bd3ba9cdb4693b3134f8519f6d.123fe6f46a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Si</t>
@@ -333,13 +333,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-10-12T14:47:18:00Z</t>
-  </si>
-  <si>
-    <t>147ebbda3906cac3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.801d325d3027b464d1db4e5495ea0b5e952d9150cc84acb2d031010f87f28aa2.e45471a5ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-10-18T13:13:25:00Z</t>
+  </si>
+  <si>
+    <t>77126b23ab9d7f96</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.812d16869f3171178394d5957a9d4b9fe359a3bd3ba9cdb4693b3134f8519f6d.8086d08d23^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT3</t>
@@ -2647,13 +2647,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-10-12T16:22:43:00</t>
-  </si>
-  <si>
-    <t>a55cf6207c8ce99a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.801d325d3027b464d1db4e5495ea0b5e952d9150cc84acb2d031010f87f28aa2.569b1ee20f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-10-18T13:05:55:00Z</t>
+  </si>
+  <si>
+    <t>fc0c8da45e8823eb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.812d16869f3171178394d5957a9d4b9fe359a3bd3ba9cdb4693b3134f8519f6d.5701ba1cf1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">ID TEST CASE OK</t>
@@ -2858,22 +2858,18 @@
     </font>
     <font>
       <sz val="14.000000"/>
-      <color indexed="64"/>
       <name val="Times New Roman"/>
     </font>
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Arial Unicode MS"/>
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Arial Unicode MS"/>
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Times New Roman"/>
     </font>
   </fonts>
@@ -2928,108 +2924,108 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="none"/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="none"/>
       <diagonal style="none"/>
@@ -3037,17 +3033,17 @@
     <border>
       <left style="none"/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="none"/>
@@ -3057,7 +3053,7 @@
     <border>
       <left style="none"/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="none"/>
       <bottom style="none"/>
@@ -3065,35 +3061,35 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="none"/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="none"/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="none"/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color indexed="65"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="none"/>
       <diagonal style="none"/>
@@ -3106,46 +3102,46 @@
         <color indexed="65"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="none"/>
       <diagonal style="none"/>
@@ -6135,7 +6131,7 @@
       <selection activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="12" width="11.42578125"/>
     <col customWidth="1" min="2" max="2" style="12" width="46.85546875"/>

</xml_diff>